<commit_message>
Huso horario al reporte : evaluaciones por modulo
</commit_message>
<xml_diff>
--- a/docs/formatos/evaluacionesModulo.xlsx
+++ b/docs/formatos/evaluacionesModulo.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22609"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\wamp\www\formacion2.0\docs\formatos\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{69544C0C-BEA9-4526-9C04-159EE751D07D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7620" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -17,21 +18,35 @@
   <definedNames>
     <definedName name="USUARIOS_20150209" localSheetId="0">Hoja1!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191028" calcCompleted="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="22">
   <si>
     <t>Evaluaciones por módulo. Desde DD/MM/AAAA. Hasta DD/MM/AAAA.</t>
   </si>
   <si>
+    <t>Empresa: YYYYYYYYYY. Programa: Pensamiento estratégico</t>
+  </si>
+  <si>
+    <t>Código</t>
+  </si>
+  <si>
     <t>Usuario</t>
   </si>
   <si>
@@ -41,6 +56,12 @@
     <t>Apellido</t>
   </si>
   <si>
+    <t>Fecha de Registro</t>
+  </si>
+  <si>
+    <t>Hora de Registro</t>
+  </si>
+  <si>
     <t>Correo</t>
   </si>
   <si>
@@ -81,22 +102,13 @@
   </si>
   <si>
     <t>Hora Presentación</t>
-  </si>
-  <si>
-    <t>Empresa: YYYYYYYYYY. Programa: Pensamiento estratégico</t>
-  </si>
-  <si>
-    <t>Código</t>
-  </si>
-  <si>
-    <t>Fecha de Registro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="5">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -481,31 +493,31 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:T5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
-      <selection activeCell="D30" sqref="D30"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="69" zoomScaleNormal="69" workbookViewId="0">
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="12.7109375" customWidth="1"/>
-    <col min="2" max="4" width="20.7109375" customWidth="1"/>
-    <col min="5" max="5" width="15.7109375" customWidth="1"/>
-    <col min="6" max="6" width="30.7109375" customWidth="1"/>
-    <col min="7" max="8" width="20.7109375" customWidth="1"/>
-    <col min="9" max="12" width="15.7109375" customWidth="1"/>
-    <col min="13" max="13" width="17.7109375" customWidth="1"/>
-    <col min="14" max="14" width="16.7109375" customWidth="1"/>
-    <col min="15" max="15" width="60.7109375" customWidth="1"/>
-    <col min="16" max="16" width="15.7109375" customWidth="1"/>
-    <col min="17" max="17" width="8.7109375" customWidth="1"/>
-    <col min="18" max="18" width="17.7109375" customWidth="1"/>
-    <col min="19" max="19" width="16.7109375" customWidth="1"/>
+    <col min="2" max="5" width="20.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
+    <col min="7" max="7" width="30.7109375" customWidth="1"/>
+    <col min="8" max="9" width="20.7109375" customWidth="1"/>
+    <col min="10" max="13" width="15.7109375" customWidth="1"/>
+    <col min="14" max="14" width="17.7109375" customWidth="1"/>
+    <col min="15" max="15" width="16.7109375" customWidth="1"/>
+    <col min="16" max="16" width="60.7109375" customWidth="1"/>
+    <col min="17" max="17" width="15.7109375" customWidth="1"/>
+    <col min="18" max="18" width="8.7109375" customWidth="1"/>
+    <col min="19" max="19" width="17.7109375" customWidth="1"/>
+    <col min="20" max="20" width="16.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:20" ht="20.25">
       <c r="A1" s="11" t="s">
         <v>0</v>
       </c>
@@ -527,10 +539,11 @@
       <c r="Q1" s="11"/>
       <c r="R1" s="11"/>
       <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
     </row>
-    <row r="2" spans="1:19" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:20" ht="20.25">
       <c r="A2" s="11" t="s">
-        <v>18</v>
+        <v>1</v>
       </c>
       <c r="B2" s="11"/>
       <c r="C2" s="11"/>
@@ -550,8 +563,9 @@
       <c r="Q2" s="11"/>
       <c r="R2" s="11"/>
       <c r="S2" s="11"/>
+      <c r="T2" s="11"/>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:20">
       <c r="B3" s="3"/>
       <c r="C3" s="3"/>
       <c r="D3" s="3"/>
@@ -570,91 +584,96 @@
       <c r="Q3" s="3"/>
       <c r="R3" s="3"/>
       <c r="S3" s="3"/>
+      <c r="T3" s="3"/>
     </row>
-    <row r="4" spans="1:19" s="2" customFormat="1" ht="39.950000000000003" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:20" s="2" customFormat="1" ht="39.950000000000003" customHeight="1">
       <c r="A4" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="C4" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="E4" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="H4" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>10</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="K4" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="L4" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="M4" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="O4" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="P4" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="Q4" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="R4" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="4" t="s">
-        <v>1</v>
-      </c>
-      <c r="C4" s="5" t="s">
-        <v>2</v>
-      </c>
-      <c r="D4" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="E4" s="5" t="s">
+      <c r="S4" s="5" t="s">
         <v>20</v>
       </c>
-      <c r="F4" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="G4" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="5" t="s">
-        <v>6</v>
-      </c>
-      <c r="I4" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="J4" s="5" t="s">
-        <v>8</v>
-      </c>
-      <c r="K4" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="L4" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="N4" s="6" t="s">
-        <v>12</v>
-      </c>
-      <c r="O4" s="6" t="s">
-        <v>13</v>
-      </c>
-      <c r="P4" s="6" t="s">
-        <v>14</v>
-      </c>
-      <c r="Q4" s="5" t="s">
-        <v>15</v>
-      </c>
-      <c r="R4" s="5" t="s">
-        <v>16</v>
-      </c>
-      <c r="S4" s="5" t="s">
-        <v>17</v>
+      <c r="T4" s="5" t="s">
+        <v>21</v>
       </c>
     </row>
-    <row r="5" spans="1:19" s="1" customFormat="1" ht="35.1" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:20" s="1" customFormat="1" ht="35.1" customHeight="1">
       <c r="A5" s="8"/>
       <c r="B5" s="7"/>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="10"/>
-      <c r="G5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="10"/>
       <c r="H5" s="7"/>
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
       <c r="K5" s="7"/>
       <c r="L5" s="7"/>
-      <c r="M5" s="8"/>
+      <c r="M5" s="7"/>
       <c r="N5" s="8"/>
-      <c r="O5" s="9"/>
-      <c r="P5" s="7"/>
+      <c r="O5" s="8"/>
+      <c r="P5" s="9"/>
       <c r="Q5" s="7"/>
-      <c r="R5" s="8"/>
+      <c r="R5" s="7"/>
       <c r="S5" s="8"/>
+      <c r="T5" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="2">
-    <mergeCell ref="A1:S1"/>
-    <mergeCell ref="A2:S2"/>
+    <mergeCell ref="A1:T1"/>
+    <mergeCell ref="A2:T2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>